<commit_message>
pdfs das instruções das iterações
</commit_message>
<xml_diff>
--- a/Banco_Imobiliario/Tabuleiro-Valores.xlsx
+++ b/Banco_Imobiliario/Tabuleiro-Valores.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Leblon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SORTE OU REVES</t>
   </si>
   <si>
     <t xml:space="preserve">Av. Presidente Vargas</t>
@@ -143,12 +146,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -171,13 +175,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -282,56 +280,60 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -518,58 +520,58 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>-200</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>60</v>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>60</v>
       </c>
     </row>
@@ -577,245 +579,293 @@
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="0" t="n">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="n">
         <v>240</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="0" t="n">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="0" t="n">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="n">
         <v>220</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="0" t="n">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="n">
         <v>220</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="0" t="n">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="0" t="n">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="0" t="n">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="0" t="n">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="n">
         <v>350</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="0" t="n">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="n">
         <v>-200</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>120</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>150</v>
+      <c r="C23" s="1" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>160</v>
+      <c r="A24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>140</v>
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>140</v>
+      <c r="A26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="0" t="n">
-        <v>0</v>
+      <c r="A27" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="0" t="n">
-        <v>260</v>
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>160</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>200</v>
+      <c r="A29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>320</v>
+        <v>28</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>140</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>300</v>
+        <v>29</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>140</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="0" t="n">
+      <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="1" t="n">
         <v>200</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="0" t="n">
-        <v>280</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C40" s="1" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="1" t="n">
         <v>260</v>
       </c>
     </row>

</xml_diff>